<commit_message>
Add code inclusion and Exclusion criteria
</commit_message>
<xml_diff>
--- a/Inputs/Diagnosis/Diseases_of_interest.xlsx
+++ b/Inputs/Diagnosis/Diseases_of_interest.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unimelbcloud-my.sharepoint.com/personal/hjameei_student_unimelb_edu_au/Documents/PhD research/UK Biobank/HETEROGENEITY/Inputs/Diagnosis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mq669/Dropbox (Partners HealthCare)/DOCUMENTS/POSTDOC_MNC/NHMRC Investigator grant/DATA MANAGEMENT/HETEROGENEITY2/Heterogeneity/Inputs/Diagnosis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="13_ncr:1_{72EE129A-1A2A-9044-8419-07230217D9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D4F02D7-904D-3242-B840-20BFFB6ADD7D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17C5146-8FC6-7C43-8272-942C6D09C2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{F85C8D89-C5F4-9242-8168-3FF0EC4F5C59}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="2" xr2:uid="{F85C8D89-C5F4-9242-8168-3FF0EC4F5C59}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Include_desc" sheetId="1" r:id="rId1"/>
+    <sheet name="Exclude_code_icd9" sheetId="2" r:id="rId2"/>
+    <sheet name="Include_codes_icd9" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="236">
   <si>
     <t>Label</t>
   </si>
@@ -398,9 +400,6 @@
     <t>Ischaemic heart</t>
   </si>
   <si>
-    <t>CKD, Chronic kidney disease</t>
-  </si>
-  <si>
     <t>bronchial</t>
   </si>
   <si>
@@ -521,9 +520,6 @@
     <t>Coronary artery disease</t>
   </si>
   <si>
-    <t>CAD</t>
-  </si>
-  <si>
     <t>coronay heart disease</t>
   </si>
   <si>
@@ -651,13 +647,112 @@
   </si>
   <si>
     <t>phobic neurosis</t>
+  </si>
+  <si>
+    <t>ANGINA PECTORIS</t>
+  </si>
+  <si>
+    <t>CORONARY ATHEROSCLEROSIS</t>
+  </si>
+  <si>
+    <t>ANEURYSM OF HEART</t>
+  </si>
+  <si>
+    <t>ISCHAEMIA, MYOCARDIAL (CHRONIC)</t>
+  </si>
+  <si>
+    <t>HYPERTENSIVE HEART DISEASE</t>
+  </si>
+  <si>
+    <t>MALIGNANT HYPERTENSIVE HEART DISEASE</t>
+  </si>
+  <si>
+    <t>BENIGN HYPERTENSIVE HEART DISEASE</t>
+  </si>
+  <si>
+    <t>HYPERTENSIVE HEART DISEASE NOT SPECIFIED</t>
+  </si>
+  <si>
+    <t>HYPERTENSIVE RENAL DISEASE</t>
+  </si>
+  <si>
+    <t>MALIGNANT HYPERTENSIVE RENAL DISEASE</t>
+  </si>
+  <si>
+    <t>BENIGN HYPERTENSIVE RENAL DISEASE</t>
+  </si>
+  <si>
+    <t>HYPERTENSIVE RENAL DISEASE NOT SPECIFIED</t>
+  </si>
+  <si>
+    <t>HYPERTENSIVE HEART AND RENAL DISEASE</t>
+  </si>
+  <si>
+    <t>MALIGNANT HYPERTENSIVE HEART AND RENAL DISEASE</t>
+  </si>
+  <si>
+    <t>BENIGN HYPERTENSIVE HEART AND RENAL DISEASE</t>
+  </si>
+  <si>
+    <t>HYPERTENSIVE HEART AND RENAL DISEASE NOT SPECIFIED</t>
+  </si>
+  <si>
+    <t>CHRONIC AIRWAYS OBSTRUCTION, NOT ELSEWHERE CLASSIFIED</t>
+  </si>
+  <si>
+    <t>CHRONIC RENAL FAILURE</t>
+  </si>
+  <si>
+    <t>Code1</t>
+  </si>
+  <si>
+    <t>Code2</t>
+  </si>
+  <si>
+    <t>Code3</t>
+  </si>
+  <si>
+    <t>Code4</t>
+  </si>
+  <si>
+    <t>Code5</t>
+  </si>
+  <si>
+    <t>Code6</t>
+  </si>
+  <si>
+    <t>Code7</t>
+  </si>
+  <si>
+    <t>715</t>
+  </si>
+  <si>
+    <t>7150</t>
+  </si>
+  <si>
+    <t>7151</t>
+  </si>
+  <si>
+    <t>7152</t>
+  </si>
+  <si>
+    <t>7153</t>
+  </si>
+  <si>
+    <t>7158</t>
+  </si>
+  <si>
+    <t>7159</t>
+  </si>
+  <si>
+    <t>9457E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -713,6 +808,11 @@
       <color theme="1"/>
       <name val="ArialMT"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -752,7 +852,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -770,6 +870,23 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1086,10 +1203,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F68461-33BF-1243-84F8-416A85DF0858}">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:R48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView topLeftCell="D8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1147,7 +1264,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1178,10 +1295,10 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1201,13 +1318,13 @@
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="H5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1224,7 +1341,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1241,10 +1358,10 @@
         <v>42</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1261,10 +1378,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1281,22 +1398,22 @@
         <v>43</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" t="s">
         <v>132</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1313,16 +1430,16 @@
         <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="G10" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1339,10 +1456,10 @@
         <v>7</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F11" t="s">
         <v>140</v>
-      </c>
-      <c r="F11" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1353,7 +1470,7 @@
         <v>90</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>44</v>
@@ -1362,7 +1479,7 @@
         <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1411,7 +1528,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1428,18 +1545,18 @@
         <v>94</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F15" t="s">
         <v>145</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="4" t="s">
-        <v>120</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>91</v>
@@ -1453,8 +1570,11 @@
       <c r="E16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="F16" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1468,16 +1588,16 @@
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" s="4" t="s">
         <v>33</v>
       </c>
@@ -1491,16 +1611,16 @@
         <v>46</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19" s="5" t="s">
         <v>11</v>
       </c>
@@ -1511,7 +1631,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:18">
       <c r="A20" s="4" t="s">
         <v>34</v>
       </c>
@@ -1525,13 +1645,13 @@
         <v>34</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21" s="4" t="s">
         <v>35</v>
       </c>
@@ -1545,16 +1665,16 @@
         <v>47</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" t="s">
         <v>157</v>
       </c>
-      <c r="G21" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22" s="4" t="s">
         <v>12</v>
       </c>
@@ -1568,10 +1688,10 @@
         <v>12</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23" s="4" t="s">
         <v>36</v>
       </c>
@@ -1594,16 +1714,25 @@
         <v>48</v>
       </c>
       <c r="H23" t="s">
+        <v>159</v>
+      </c>
+      <c r="I23" t="s">
         <v>160</v>
       </c>
-      <c r="I23" t="s">
-        <v>161</v>
-      </c>
-      <c r="J23" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="J23" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="K23" t="s">
+        <v>204</v>
+      </c>
+      <c r="L23" t="s">
+        <v>205</v>
+      </c>
+      <c r="M23" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
@@ -1620,10 +1749,46 @@
         <v>50</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+        <v>161</v>
+      </c>
+      <c r="G24" t="s">
+        <v>207</v>
+      </c>
+      <c r="H24" t="s">
+        <v>208</v>
+      </c>
+      <c r="I24" t="s">
+        <v>209</v>
+      </c>
+      <c r="J24" t="s">
+        <v>210</v>
+      </c>
+      <c r="K24" t="s">
+        <v>211</v>
+      </c>
+      <c r="L24" t="s">
+        <v>212</v>
+      </c>
+      <c r="M24" t="s">
+        <v>213</v>
+      </c>
+      <c r="N24" t="s">
+        <v>214</v>
+      </c>
+      <c r="O24" t="s">
+        <v>215</v>
+      </c>
+      <c r="P24" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>217</v>
+      </c>
+      <c r="R24" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25" s="4" t="s">
         <v>13</v>
       </c>
@@ -1646,7 +1811,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:18">
       <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
@@ -1671,8 +1836,11 @@
       <c r="H26" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="I26" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
       <c r="A27" s="4" t="s">
         <v>16</v>
       </c>
@@ -1686,13 +1854,13 @@
         <v>16</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28" s="4" t="s">
         <v>17</v>
       </c>
@@ -1706,7 +1874,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:18">
       <c r="A29" s="4" t="s">
         <v>18</v>
       </c>
@@ -1720,30 +1888,30 @@
         <v>18</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F29" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
       <c r="A30" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E30" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
       <c r="A31" s="4" t="s">
         <v>20</v>
       </c>
@@ -1757,10 +1925,10 @@
         <v>20</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
       <c r="A32" s="4" t="s">
         <v>21</v>
       </c>
@@ -1774,10 +1942,10 @@
         <v>21</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1794,19 +1962,19 @@
         <v>87</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1820,19 +1988,19 @@
         <v>80</v>
       </c>
       <c r="D34" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F34" s="8" t="s">
+      <c r="H34" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1849,10 +2017,10 @@
         <v>23</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1869,7 +2037,7 @@
         <v>24</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1903,13 +2071,13 @@
         <v>39</v>
       </c>
       <c r="E38" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1926,10 +2094,10 @@
         <v>54</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1946,13 +2114,13 @@
         <v>25</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="G40" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1992,13 +2160,13 @@
         <v>60</v>
       </c>
       <c r="E42" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G42" t="s">
         <v>195</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="G42" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -2021,13 +2189,13 @@
         <v>64</v>
       </c>
       <c r="G43" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H43" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="H43" s="7" t="s">
-        <v>200</v>
-      </c>
       <c r="I43" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -2061,7 +2229,7 @@
         <v>67</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -2078,10 +2246,10 @@
         <v>26</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -2118,8 +2286,1551 @@
         <v>112</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>202</v>
-      </c>
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C395F5C-21C5-E243-9639-329C23993E2C}">
+  <dimension ref="A1:H48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="26">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="13"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="9">
+        <v>9920</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="C26" s="10">
+        <v>9757</v>
+      </c>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="11"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="11"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E15FE0-283C-E243-B347-54FE2E84EFF2}">
+  <dimension ref="A1:O50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="3" customFormat="1" ht="26">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" t="s">
+        <v>228</v>
+      </c>
+      <c r="C29" t="s">
+        <v>229</v>
+      </c>
+      <c r="D29" t="s">
+        <v>230</v>
+      </c>
+      <c r="E29" t="s">
+        <v>231</v>
+      </c>
+      <c r="F29" t="s">
+        <v>232</v>
+      </c>
+      <c r="G29" t="s">
+        <v>233</v>
+      </c>
+      <c r="H29" t="s">
+        <v>234</v>
+      </c>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="10"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
+      <c r="N38" s="11"/>
+      <c r="O38" s="11"/>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="10"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="11"/>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="11"/>
+      <c r="O40" s="11"/>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="10"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="11"/>
+      <c r="O41" s="11"/>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="A42" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11"/>
+      <c r="O42" s="11"/>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="A43" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43" s="10"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11"/>
+      <c r="O43" s="11"/>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="10"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="11"/>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="A46" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="11"/>
+      <c r="O46" s="11"/>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="A47" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="10"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="11"/>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="A48" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="11"/>
+      <c r="O48" s="11"/>
+    </row>
+    <row r="49" spans="2:15">
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11"/>
+      <c r="N49" s="11"/>
+      <c r="O49" s="11"/>
+    </row>
+    <row r="50" spans="2:15">
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="11"/>
+      <c r="M50" s="11"/>
+      <c r="N50" s="11"/>
+      <c r="O50" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
deleted organ column from include/exclude
</commit_message>
<xml_diff>
--- a/Inputs/Diagnosis/Diseases_of_interest.xlsx
+++ b/Inputs/Diagnosis/Diseases_of_interest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unimelbcloud-my.sharepoint.com/personal/hjameei_student_unimelb_edu_au/Documents/PhD research/UK Biobank/Heterogeneity/Inputs/Diagnosis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{EFD40B4E-CDED-7B4E-B2F5-3C8175F54896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70DF355A-BCBF-C74F-88C5-C615B9556201}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{EFD40B4E-CDED-7B4E-B2F5-3C8175F54896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16713615-7CA2-F64B-A9C1-22A04DC64A21}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="760" windowWidth="33600" windowHeight="20500" activeTab="6" xr2:uid="{F85C8D89-C5F4-9242-8168-3FF0EC4F5C59}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="291">
   <si>
     <t>Label</t>
   </si>
@@ -2435,608 +2435,465 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C395F5C-21C5-E243-9639-329C23993E2C}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.5" customWidth="1"/>
-    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="26">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="26">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>73</v>
+        <v>211</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="I1" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:9">
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="B7" s="1"/>
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:9">
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:9">
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>77</v>
+      <c r="B10" t="s">
+        <v>229</v>
       </c>
       <c r="C10" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D10" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E10" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F10" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H10" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:9">
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:9">
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:9">
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B15" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:8">
       <c r="A16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-    </row>
-    <row r="17" spans="1:9">
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>82</v>
+      <c r="B17" t="s">
+        <v>250</v>
       </c>
       <c r="C17" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E17" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:8">
       <c r="A18" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:9">
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C19" s="1">
+      <c r="B19" s="1">
         <v>7792</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="C19" s="1"/>
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B20" t="s">
         <v>287</v>
       </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:9">
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-    </row>
-    <row r="22" spans="1:9">
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>82</v>
+      <c r="B22" t="s">
+        <v>282</v>
       </c>
       <c r="C22" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D22" t="s">
-        <v>283</v>
-      </c>
-      <c r="E22" t="s">
         <v>284</v>
       </c>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:9">
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="I25" s="8"/>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="B25" s="1"/>
+      <c r="H25" s="8"/>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" s="8">
+      <c r="B26" s="8">
         <v>9920</v>
       </c>
+      <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:9">
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:9">
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>88</v>
-      </c>
+      <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="9"/>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>88</v>
+      <c r="B31" t="s">
+        <v>275</v>
       </c>
       <c r="C31" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D31" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E31" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F31" t="s">
-        <v>278</v>
-      </c>
-      <c r="G31" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:8">
       <c r="A32" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>88</v>
-      </c>
+      <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:7">
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>86</v>
-      </c>
+      <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="1:7">
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>76</v>
+      <c r="B35" t="s">
+        <v>225</v>
       </c>
       <c r="C35" t="s">
-        <v>225</v>
-      </c>
-      <c r="D35" t="s">
         <v>271</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="D35" s="11" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:6">
       <c r="A36" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C37" s="8" t="s">
+      <c r="B37" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="D37" s="1">
+      <c r="C37" s="1">
         <v>9757</v>
       </c>
+      <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7">
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>94</v>
+      <c r="B38" t="s">
+        <v>269</v>
       </c>
       <c r="C38" t="s">
-        <v>269</v>
-      </c>
-      <c r="D38" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:6">
       <c r="A39" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:7">
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C40" s="1"/>
-      <c r="E40" s="9"/>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="B40" s="1"/>
+      <c r="D40" s="9"/>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-    </row>
-    <row r="42" spans="1:7">
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:7">
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="B43" s="1"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-    </row>
-    <row r="44" spans="1:7">
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C44" s="1"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="10"/>
-    </row>
-    <row r="45" spans="1:7">
+      <c r="B44" s="1"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="10"/>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C46" s="1"/>
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="1:7">
+      <c r="B46" s="1"/>
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>97</v>
-      </c>
+      <c r="B47" s="1"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="9"/>
+      <c r="D47" s="9"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I47">
-    <sortCondition ref="B2:B47"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H47">
     <sortCondition ref="A2:A47"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -3046,664 +2903,521 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E15FE0-283C-E243-B347-54FE2E84EFF2}">
-  <dimension ref="A1:P47"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:XFD1048576"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.5" customWidth="1"/>
-    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="26">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="26">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>73</v>
+        <v>211</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="I1" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:9">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>77</v>
+      <c r="B6" t="s">
+        <v>228</v>
       </c>
       <c r="C6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D6" t="s">
-        <v>226</v>
-      </c>
-      <c r="E6" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="B7" s="1"/>
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:9">
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:9">
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:9">
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:9">
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:9">
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-    </row>
-    <row r="17" spans="1:16">
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>82</v>
+      <c r="B17" t="s">
+        <v>253</v>
       </c>
       <c r="C17" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D17" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E17" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F17" t="s">
-        <v>256</v>
-      </c>
-      <c r="G17" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:15">
       <c r="A18" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:16">
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B19" t="s">
         <v>249</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="C19" s="1"/>
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:16">
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-    </row>
-    <row r="22" spans="1:16">
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:16">
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>82</v>
+      <c r="B23" t="s">
+        <v>235</v>
       </c>
       <c r="C23" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D23" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E23" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F23" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G23" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H23" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="I23" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="J23" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="K23" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="L23" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="M23" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="N23" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="O23" t="s">
-        <v>247</v>
-      </c>
-      <c r="P23" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:15">
       <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:16">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="I25" s="8"/>
-    </row>
-    <row r="26" spans="1:16">
+      <c r="B25" s="1"/>
+      <c r="H25" s="8"/>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>105</v>
-      </c>
+      <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:16">
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:16">
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C28">
+      <c r="B28">
         <v>7193</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:15">
       <c r="A29" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:16">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>88</v>
-      </c>
+      <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="9"/>
-    </row>
-    <row r="31" spans="1:16">
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>88</v>
-      </c>
+      <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>88</v>
-      </c>
+      <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:13">
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C34" s="1"/>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="B34" s="1"/>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>76</v>
-      </c>
+      <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-    </row>
-    <row r="36" spans="1:13">
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>92</v>
-      </c>
+      <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:13">
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>94</v>
+      <c r="B38" t="s">
+        <v>258</v>
       </c>
       <c r="C38" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D38" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E38" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F38" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="G38" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="H38" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="I38" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="J38" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="K38" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="L38" t="s">
-        <v>267</v>
-      </c>
-      <c r="M38" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:12">
       <c r="A39" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:13">
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C40" s="1"/>
-      <c r="E40" s="9"/>
-    </row>
-    <row r="41" spans="1:13">
+      <c r="B40" s="1"/>
+      <c r="D40" s="9"/>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>94</v>
+      <c r="B41" t="s">
+        <v>218</v>
       </c>
       <c r="C41" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D41" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E41" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F41" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G41" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H41" t="s">
-        <v>223</v>
-      </c>
-      <c r="I41" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:12">
       <c r="A42" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="9"/>
-    </row>
-    <row r="43" spans="1:13">
+      <c r="D42" s="9"/>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-    </row>
-    <row r="44" spans="1:13">
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C44" s="1"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="10"/>
-    </row>
-    <row r="45" spans="1:13">
+      <c r="B44" s="1"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="10"/>
+    </row>
+    <row r="45" spans="1:12">
       <c r="A45" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>174</v>
+      <c r="B45" t="s">
+        <v>226</v>
       </c>
       <c r="C45" t="s">
-        <v>226</v>
-      </c>
-      <c r="D45" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:12">
       <c r="A46" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>87</v>
-      </c>
+      <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-    </row>
-    <row r="47" spans="1:13">
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>97</v>
-      </c>
+      <c r="B47" s="1"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P47">
-    <sortCondition ref="B2:B47"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O47">
     <sortCondition ref="A2:A47"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -3713,424 +3427,281 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8016D5CD-B4CE-1540-83E9-1BF3C2D05B33}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="A1:XFD1048576"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="48.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26">
+    <row r="1" spans="1:8" ht="26">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>73</v>
+        <v>211</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="I1" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17">
+      <c r="B17">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:2">
       <c r="A18" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22">
+      <c r="B22">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:2">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+    </row>
+    <row r="33" spans="1:1">
       <c r="A33" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+    </row>
+    <row r="34" spans="1:1">
       <c r="A34" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+    </row>
+    <row r="35" spans="1:1">
       <c r="A35" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+    </row>
+    <row r="36" spans="1:1">
       <c r="A36" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+    </row>
+    <row r="37" spans="1:1">
       <c r="A37" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+    </row>
+    <row r="38" spans="1:1">
       <c r="A38" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+    </row>
+    <row r="39" spans="1:1">
       <c r="A39" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
+    </row>
+    <row r="40" spans="1:1">
       <c r="A40" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+    </row>
+    <row r="41" spans="1:1">
       <c r="A41" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+    </row>
+    <row r="42" spans="1:1">
       <c r="A42" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+    </row>
+    <row r="43" spans="1:1">
       <c r="A43" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
+    </row>
+    <row r="44" spans="1:1">
       <c r="A44" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
+    </row>
+    <row r="45" spans="1:1">
       <c r="A45" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+    </row>
+    <row r="46" spans="1:1">
       <c r="A46" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
+    </row>
+    <row r="47" spans="1:1">
       <c r="A47" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>97</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I47">
-    <sortCondition ref="B2:B47"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H47">
     <sortCondition ref="A2:A47"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4139,421 +3710,278 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A118984D-C662-2241-AA55-5D3B89E5856E}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="A1:I47"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="48.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26">
+    <row r="1" spans="1:8" ht="26">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>73</v>
+        <v>211</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="I1" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C19">
+      <c r="B19">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:2">
       <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+    </row>
+    <row r="33" spans="1:1">
       <c r="A33" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+    </row>
+    <row r="34" spans="1:1">
       <c r="A34" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+    </row>
+    <row r="35" spans="1:1">
       <c r="A35" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+    </row>
+    <row r="36" spans="1:1">
       <c r="A36" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+    </row>
+    <row r="37" spans="1:1">
       <c r="A37" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+    </row>
+    <row r="38" spans="1:1">
       <c r="A38" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+    </row>
+    <row r="39" spans="1:1">
       <c r="A39" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
+    </row>
+    <row r="40" spans="1:1">
       <c r="A40" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+    </row>
+    <row r="41" spans="1:1">
       <c r="A41" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+    </row>
+    <row r="42" spans="1:1">
       <c r="A42" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+    </row>
+    <row r="43" spans="1:1">
       <c r="A43" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
+    </row>
+    <row r="44" spans="1:1">
       <c r="A44" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
+    </row>
+    <row r="45" spans="1:1">
       <c r="A45" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+    </row>
+    <row r="46" spans="1:1">
       <c r="A46" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
+    </row>
+    <row r="47" spans="1:1">
       <c r="A47" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>97</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I47">
-    <sortCondition ref="B2:B47"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H47">
     <sortCondition ref="A2:A47"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4562,526 +3990,383 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB4C7C3-CF9C-7644-8AB7-9F7315D08EEE}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="B13" sqref="A1:I47"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="41.5" customWidth="1"/>
-    <col min="2" max="2" width="46.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26">
+    <row r="1" spans="1:8" ht="26">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>73</v>
+        <v>211</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="I1" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:9">
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="B7" s="1"/>
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:9">
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:9">
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:9">
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:9">
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:9">
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-    </row>
-    <row r="17" spans="1:9">
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:9">
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:9">
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-    </row>
-    <row r="22" spans="1:9">
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:9">
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="I25" s="8"/>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="B25" s="1"/>
+      <c r="H25" s="8"/>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:9">
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:9">
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>88</v>
-      </c>
+      <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="9"/>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>88</v>
-      </c>
+      <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:7">
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>86</v>
-      </c>
+      <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="1:7">
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E35" s="11"/>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="D35" s="11"/>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7">
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:7">
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C40" s="1"/>
-      <c r="E40" s="9"/>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="B40" s="1"/>
+      <c r="D40" s="9"/>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-    </row>
-    <row r="42" spans="1:7">
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:7">
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="B43" s="1"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-    </row>
-    <row r="44" spans="1:7">
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C44" s="1"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="10"/>
-    </row>
-    <row r="45" spans="1:7">
+      <c r="B44" s="1"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="10"/>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C46" s="1"/>
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="1:7">
+      <c r="B46" s="1"/>
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>97</v>
-      </c>
+      <c r="B47" s="1"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="9"/>
+      <c r="D47" s="9"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I47">
-    <sortCondition ref="B2:B47"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H47">
     <sortCondition ref="A2:A47"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5090,524 +4375,379 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA1A1CFA-EA26-0A45-AB9C-3D3BEC3C727E}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:XFD1048576"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="2" max="2" width="46.5" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26">
+    <row r="1" spans="1:8" ht="26">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>73</v>
+        <v>211</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="I1" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:9">
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="B7" s="1"/>
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:9">
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:9">
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:9">
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:9">
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:9">
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-    </row>
-    <row r="17" spans="1:9">
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:9">
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:9">
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-    </row>
-    <row r="22" spans="1:9">
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:9">
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="I25" s="8"/>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="B25" s="1"/>
+      <c r="H25" s="8"/>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:9">
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:9">
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>88</v>
-      </c>
+      <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="9"/>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>88</v>
-      </c>
+      <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:7">
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>86</v>
-      </c>
+      <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="1:7">
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7">
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:7">
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C40" s="1"/>
-      <c r="E40" s="9"/>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="B40" s="1"/>
+      <c r="D40" s="9"/>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-    </row>
-    <row r="42" spans="1:7">
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:7">
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="B43" s="1"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-    </row>
-    <row r="44" spans="1:7">
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C44" s="1"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="10"/>
-    </row>
-    <row r="45" spans="1:7">
+      <c r="B44" s="1"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="10"/>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C46" s="1"/>
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="1:7">
+      <c r="B46" s="1"/>
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>97</v>
-      </c>
+      <c r="B47" s="1"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="9"/>
+      <c r="D47" s="9"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I47">
-    <sortCondition ref="B2:B47"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H47">
     <sortCondition ref="A2:A47"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Diagnostic workflow amendments with error
</commit_message>
<xml_diff>
--- a/Inputs/Diagnosis/Diseases_of_interest.xlsx
+++ b/Inputs/Diagnosis/Diseases_of_interest.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unimelbcloud-my.sharepoint.com/personal/hjameei_student_unimelb_edu_au/Documents/PhD research/UK Biobank/Heterogeneity/Inputs/Diagnosis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mq669/Dropbox (Partners HealthCare)/DOCUMENTS/POSTDOC_MNC/NHMRC Investigator grant/DATA MANAGEMENT/HETEROGENEITY2/Heterogeneity/Inputs/Diagnosis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="283" documentId="13_ncr:1_{EFD40B4E-CDED-7B4E-B2F5-3C8175F54896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A047AFA-BC07-7D41-80E0-8F6B2E41FF37}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D48D522-55F1-D648-B884-732CD5CCE9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="760" windowWidth="33600" windowHeight="20500" activeTab="6" xr2:uid="{F85C8D89-C5F4-9242-8168-3FF0EC4F5C59}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{F85C8D89-C5F4-9242-8168-3FF0EC4F5C59}"/>
   </bookViews>
   <sheets>
     <sheet name="Include_desc" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="463">
   <si>
     <t>Label</t>
   </si>
@@ -1919,7 +1919,7 @@
   <dimension ref="A1:R46"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2967,8 +2967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E15FE0-283C-E243-B347-54FE2E84EFF2}">
   <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView zoomScale="142" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="142" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3332,9 +3332,7 @@
       <c r="A36" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>297</v>
-      </c>
+      <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -3481,8 +3479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C395F5C-21C5-E243-9639-329C23993E2C}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3941,7 +3939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB4C7C3-CF9C-7644-8AB7-9F7315D08EEE}">
   <dimension ref="A1:AS46"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="125" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -5509,7 +5507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A118984D-C662-2241-AA55-5D3B89E5856E}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added self codes in crosscheck - yet to be tested
</commit_message>
<xml_diff>
--- a/Inputs/Diagnosis/Diseases_of_interest.xlsx
+++ b/Inputs/Diagnosis/Diseases_of_interest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unimelbcloud-my.sharepoint.com/personal/hjameei_student_unimelb_edu_au/Documents/PhD research/UK Biobank/Heterogeneity/Inputs/Diagnosis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{6D48D522-55F1-D648-B884-732CD5CCE9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{893B8B5D-EA7E-B14A-8CC5-5027D2B073C9}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{6D48D522-55F1-D648-B884-732CD5CCE9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E4058F8-EAAF-544C-9DEA-95214BC1BB2D}"/>
   <bookViews>
-    <workbookView xWindow="9420" yWindow="760" windowWidth="24180" windowHeight="20460" activeTab="2" xr2:uid="{F85C8D89-C5F4-9242-8168-3FF0EC4F5C59}"/>
+    <workbookView xWindow="100" yWindow="760" windowWidth="34460" windowHeight="20460" firstSheet="2" activeTab="4" xr2:uid="{F85C8D89-C5F4-9242-8168-3FF0EC4F5C59}"/>
   </bookViews>
   <sheets>
     <sheet name="Include_desc" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="Exclude_code_icd10" sheetId="7" r:id="rId5"/>
     <sheet name="Include_code_mhq" sheetId="5" r:id="rId6"/>
     <sheet name="Exclude_code_mhq" sheetId="4" r:id="rId7"/>
+    <sheet name="Include_code_self" sheetId="8" r:id="rId8"/>
+    <sheet name="Exclude_code_self" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="B21.0" localSheetId="3">Include_code_icd10!$B$37</definedName>
@@ -60,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="477">
   <si>
     <t>Label</t>
   </si>
@@ -3528,7 +3530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C395F5C-21C5-E243-9639-329C23993E2C}">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -3997,8 +3999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB4C7C3-CF9C-7644-8AB7-9F7315D08EEE}">
   <dimension ref="A1:AS46"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="125" workbookViewId="0">
-      <selection activeCell="AS40" sqref="A40:AS40"/>
+    <sheetView topLeftCell="AN23" zoomScale="125" workbookViewId="0">
+      <selection activeCell="AV56" sqref="AV56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4600,10 +4602,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA1A1CFA-EA26-0A45-AB9C-3D3BEC3C727E}">
-  <dimension ref="A1:CF46"/>
+  <dimension ref="A1:AU46"/>
   <sheetViews>
-    <sheetView topLeftCell="BV23" workbookViewId="0">
-      <selection activeCell="CF9" sqref="A9:CF9"/>
+    <sheetView tabSelected="1" zoomScale="180" workbookViewId="0">
+      <selection activeCell="AU9" sqref="A9:AU9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4611,7 +4613,7 @@
     <col min="1" max="1" width="41.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" ht="26">
+    <row r="1" spans="1:47" ht="26">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4637,7 +4639,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:84">
+    <row r="2" spans="1:47">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -4650,7 +4652,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:84">
+    <row r="3" spans="1:47">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -4660,7 +4662,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:84">
+    <row r="4" spans="1:47">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -4670,7 +4672,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:84">
+    <row r="5" spans="1:47">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -4679,7 +4681,7 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:84">
+    <row r="6" spans="1:47">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -4688,14 +4690,14 @@
       </c>
       <c r="C6" s="9"/>
     </row>
-    <row r="7" spans="1:84">
+    <row r="7" spans="1:47">
       <c r="A7" s="4" t="s">
         <v>100</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:84">
+    <row r="8" spans="1:47">
       <c r="A8" s="4" t="s">
         <v>82</v>
       </c>
@@ -4706,7 +4708,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:84">
+    <row r="9" spans="1:47">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -4848,119 +4850,8 @@
       <c r="AU9" t="s">
         <v>406</v>
       </c>
-      <c r="AV9" t="s">
-        <v>370</v>
-      </c>
-      <c r="AW9" t="s">
-        <v>371</v>
-      </c>
-      <c r="AX9" t="s">
-        <v>372</v>
-      </c>
-      <c r="AY9" t="s">
-        <v>373</v>
-      </c>
-      <c r="AZ9" t="s">
-        <v>374</v>
-      </c>
-      <c r="BA9" t="s">
-        <v>375</v>
-      </c>
-      <c r="BB9" t="s">
-        <v>376</v>
-      </c>
-      <c r="BC9" t="s">
-        <v>377</v>
-      </c>
-      <c r="BD9" t="s">
-        <v>378</v>
-      </c>
-      <c r="BE9" t="s">
-        <v>379</v>
-      </c>
-      <c r="BF9" t="s">
-        <v>380</v>
-      </c>
-      <c r="BG9" t="s">
-        <v>381</v>
-      </c>
-      <c r="BH9" t="s">
-        <v>382</v>
-      </c>
-      <c r="BI9" t="s">
-        <v>383</v>
-      </c>
-      <c r="BJ9" t="s">
-        <v>384</v>
-      </c>
-      <c r="BK9" t="s">
-        <v>385</v>
-      </c>
-      <c r="BL9" t="s">
-        <v>386</v>
-      </c>
-      <c r="BM9" t="s">
-        <v>387</v>
-      </c>
-      <c r="BN9" t="s">
-        <v>388</v>
-      </c>
-      <c r="BO9" t="s">
-        <v>389</v>
-      </c>
-      <c r="BP9" t="s">
-        <v>390</v>
-      </c>
-      <c r="BQ9" t="s">
-        <v>391</v>
-      </c>
-      <c r="BR9" t="s">
-        <v>392</v>
-      </c>
-      <c r="BS9" t="s">
-        <v>393</v>
-      </c>
-      <c r="BT9" t="s">
-        <v>394</v>
-      </c>
-      <c r="BU9" t="s">
-        <v>395</v>
-      </c>
-      <c r="BV9" t="s">
-        <v>396</v>
-      </c>
-      <c r="BW9" t="s">
-        <v>397</v>
-      </c>
-      <c r="BX9" t="s">
-        <v>398</v>
-      </c>
-      <c r="BY9" t="s">
-        <v>399</v>
-      </c>
-      <c r="BZ9" t="s">
-        <v>400</v>
-      </c>
-      <c r="CA9" t="s">
-        <v>401</v>
-      </c>
-      <c r="CB9" t="s">
-        <v>402</v>
-      </c>
-      <c r="CC9" t="s">
-        <v>403</v>
-      </c>
-      <c r="CD9" t="s">
-        <v>404</v>
-      </c>
-      <c r="CE9" t="s">
-        <v>405</v>
-      </c>
-      <c r="CF9" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="10" spans="1:84">
+    </row>
+    <row r="10" spans="1:47">
       <c r="A10" s="4" t="s">
         <v>32</v>
       </c>
@@ -4968,13 +4859,13 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:84">
+    <row r="11" spans="1:47">
       <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:84">
+    <row r="12" spans="1:47">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
@@ -4982,14 +4873,14 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:84">
+    <row r="13" spans="1:47">
       <c r="A13" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:84">
+    <row r="14" spans="1:47">
       <c r="A14" s="4" t="s">
         <v>37</v>
       </c>
@@ -5003,7 +4894,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="15" spans="1:84">
+    <row r="15" spans="1:47">
       <c r="A15" s="4" t="s">
         <v>57</v>
       </c>
@@ -5012,7 +4903,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:84">
+    <row r="16" spans="1:47">
       <c r="A16" s="4" t="s">
         <v>81</v>
       </c>
@@ -5451,7 +5342,7 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5729,7 +5620,7 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView zoomScale="60" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="J50" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5997,4 +5888,566 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B191CA-C28A-F442-B166-7EE92FE5B688}">
+  <dimension ref="A1:H46"/>
+  <sheetViews>
+    <sheetView zoomScale="160" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="48.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="26">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24">
+        <v>1074</v>
+      </c>
+      <c r="C24">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <v>1081</v>
+      </c>
+      <c r="C25">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="12" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39">
+        <v>1065</v>
+      </c>
+      <c r="C39">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F503B91-9001-564F-BA72-B91D0D7419B8}">
+  <dimension ref="A1:H46"/>
+  <sheetViews>
+    <sheetView topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="48.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="26">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="12" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added inclusion/exclusion criteria both codes and programmed
</commit_message>
<xml_diff>
--- a/Inputs/Diagnosis/Diseases_of_interest.xlsx
+++ b/Inputs/Diagnosis/Diseases_of_interest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unimelbcloud-my.sharepoint.com/personal/hjameei_student_unimelb_edu_au/Documents/PhD research/UK Biobank/Heterogeneity/Inputs/Diagnosis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{6D48D522-55F1-D648-B884-732CD5CCE9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E4058F8-EAAF-544C-9DEA-95214BC1BB2D}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{6D48D522-55F1-D648-B884-732CD5CCE9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FFF5338-9BBB-BB48-BE68-F2C33B09337E}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="760" windowWidth="34460" windowHeight="20460" firstSheet="2" activeTab="4" xr2:uid="{F85C8D89-C5F4-9242-8168-3FF0EC4F5C59}"/>
+    <workbookView xWindow="100" yWindow="760" windowWidth="34460" windowHeight="20460" firstSheet="2" activeTab="8" xr2:uid="{F85C8D89-C5F4-9242-8168-3FF0EC4F5C59}"/>
   </bookViews>
   <sheets>
     <sheet name="Include_desc" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="487">
   <si>
     <t>Label</t>
   </si>
@@ -1493,6 +1493,36 @@
   </si>
   <si>
     <t>Y47.9</t>
+  </si>
+  <si>
+    <t>1076</t>
+  </si>
+  <si>
+    <t>1491</t>
+  </si>
+  <si>
+    <t>1192</t>
+  </si>
+  <si>
+    <t>1193</t>
+  </si>
+  <si>
+    <t>1194</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>1397</t>
+  </si>
+  <si>
+    <t>1436</t>
+  </si>
+  <si>
+    <t>1286</t>
+  </si>
+  <si>
+    <t>1291</t>
   </si>
 </sst>
 </file>
@@ -4604,7 +4634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA1A1CFA-EA26-0A45-AB9C-3D3BEC3C727E}">
   <dimension ref="A1:AU46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="180" workbookViewId="0">
       <selection activeCell="AU9" sqref="A9:AU9"/>
     </sheetView>
   </sheetViews>
@@ -5894,8 +5924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B191CA-C28A-F442-B166-7EE92FE5B688}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView zoomScale="160" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A2" zoomScale="160" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6004,45 +6034,45 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="B18" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:4">
       <c r="A21" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:4">
       <c r="A22" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:4">
       <c r="A23" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:4">
       <c r="A24" s="4" t="s">
         <v>33</v>
       </c>
@@ -6052,8 +6082,11 @@
       <c r="C24">
         <v>1075</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="4" t="s">
         <v>10</v>
       </c>
@@ -6063,38 +6096,50 @@
       <c r="C25">
         <v>1086</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:4">
       <c r="A27" s="12" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:4">
       <c r="A28" s="4" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="B28" t="s">
+        <v>479</v>
+      </c>
+      <c r="C28" t="s">
+        <v>480</v>
+      </c>
+      <c r="D28" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
         <v>14</v>
       </c>
@@ -6158,6 +6203,9 @@
     <row r="43" spans="1:3">
       <c r="A43" s="4" t="s">
         <v>13</v>
+      </c>
+      <c r="B43" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -6184,8 +6232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F503B91-9001-564F-BA72-B91D0D7419B8}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6248,11 +6296,17 @@
       <c r="A7" s="4" t="s">
         <v>100</v>
       </c>
+      <c r="B7" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="4" t="s">
         <v>82</v>
       </c>
+      <c r="B8" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="4" t="s">
@@ -6303,8 +6357,8 @@
       <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B18">
-        <v>10</v>
+      <c r="B18" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -6377,72 +6431,81 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:2">
       <c r="A33" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:2">
       <c r="A34" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:2">
       <c r="A35" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:2">
       <c r="A36" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:2">
       <c r="A37" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="B37" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:2">
       <c r="A39" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="B39" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:2">
       <c r="A41" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:2">
       <c r="A42" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:2">
       <c r="A43" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="44" spans="1:1">
+      <c r="B43" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:2">
       <c r="A45" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:2">
       <c r="A46" s="4" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Add the pre-assement diagnosis status for cancer codes Added cancer as diseases of interest
</commit_message>
<xml_diff>
--- a/Inputs/Diagnosis/Diseases_of_interest.xlsx
+++ b/Inputs/Diagnosis/Diseases_of_interest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mq669/Dropbox (Partners HealthCare)/DOCUMENTS/POSTDOC_MNC/NHMRC Investigator grant/DATA MANAGEMENT/HETEROGENEITY2/Heterogeneity/Inputs/Diagnosis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unimelbcloud-my.sharepoint.com/personal/hjameei_student_unimelb_edu_au/Documents/PhD research/UK Biobank/Heterogeneity/Inputs/Diagnosis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86456291-690D-A145-B79D-1AD3C73E647F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{86456291-690D-A145-B79D-1AD3C73E647F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0EBDD91-BE96-534A-92CC-EFD8892974A7}"/>
   <bookViews>
-    <workbookView xWindow="36560" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{F85C8D89-C5F4-9242-8168-3FF0EC4F5C59}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{F85C8D89-C5F4-9242-8168-3FF0EC4F5C59}"/>
   </bookViews>
   <sheets>
     <sheet name="Include_desc" sheetId="1" r:id="rId1"/>
@@ -6447,8 +6447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A661A7B0-6B12-E648-B675-65F23693028A}">
   <dimension ref="A1:BK160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -13281,7 +13281,9 @@
       <c r="A37" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B37" s="4"/>
+      <c r="B37" s="4">
+        <v>1</v>
+      </c>
       <c r="C37" s="4"/>
       <c r="D37" s="16" t="s">
         <v>21</v>

</xml_diff>